<commit_message>
fix bugs and add Account of customer feature
</commit_message>
<xml_diff>
--- a/src/ExcelFile/TransportTemplate/TemplateImportTransport.xlsx
+++ b/src/ExcelFile/TransportTemplate/TemplateImportTransport.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
   <si>
     <t>Loại Vận Đơn</t>
   </si>
@@ -179,27 +179,6 @@
     <t>GhiChuDP</t>
   </si>
   <si>
-    <t>FCL</t>
-  </si>
-  <si>
-    <t>CUS00001</t>
-  </si>
-  <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>CONT20</t>
-  </si>
-  <si>
-    <t>xuat</t>
-  </si>
-  <si>
-    <t>MEA</t>
-  </si>
-  <si>
-    <t>345345345989</t>
-  </si>
-  <si>
     <t>DiemDongHang</t>
   </si>
   <si>
@@ -222,13 +201,16 @@
   </si>
   <si>
     <t>Điểm Lấy Rỗng</t>
+  </si>
+  <si>
+    <t>Account</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,20 +243,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FFFF0000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,6 +254,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -315,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -323,23 +299,17 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,405 +590,236 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD8"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10" style="8" customWidth="1"/>
-    <col min="24" max="24" width="22" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.85546875" style="8" customWidth="1"/>
-    <col min="26" max="26" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10" style="7" customWidth="1"/>
+    <col min="25" max="25" width="22" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" style="7" customWidth="1"/>
+    <col min="27" max="27" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="R1" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC1" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD1" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="P2" s="12" t="s">
+      <c r="Q2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="R2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="S2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="X2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="Y2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Z2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="Z2" s="9" t="s">
+      <c r="AA2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AA2" s="9" t="s">
+      <c r="AB2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AB2" s="9" t="s">
+      <c r="AC2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="AC2" s="9" t="s">
+      <c r="AD2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AD2" s="9" t="s">
+      <c r="AE2" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="16">
-        <v>140</v>
-      </c>
-      <c r="H3" s="16">
-        <v>141</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="O3" s="17">
-        <v>140</v>
-      </c>
-      <c r="T3" s="5">
-        <v>45004.833333333336</v>
-      </c>
-      <c r="X3" s="15"/>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="W4"/>
-      <c r="X4"/>
-      <c r="Y4"/>
-      <c r="Z4"/>
-      <c r="AA4"/>
-      <c r="AB4"/>
-      <c r="AC4"/>
-      <c r="AD4"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-      <c r="N5"/>
-      <c r="O5"/>
-      <c r="P5"/>
-      <c r="Q5"/>
-      <c r="R5"/>
-      <c r="W5"/>
-      <c r="X5"/>
-      <c r="Y5"/>
-      <c r="Z5"/>
-      <c r="AA5"/>
-      <c r="AB5"/>
-      <c r="AC5"/>
-      <c r="AD5"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6"/>
-      <c r="W6"/>
-      <c r="X6"/>
-      <c r="Y6"/>
-      <c r="Z6"/>
-      <c r="AA6"/>
-      <c r="AB6"/>
-      <c r="AC6"/>
-      <c r="AD6"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-      <c r="R7"/>
-      <c r="W7"/>
-      <c r="X7"/>
-      <c r="Y7"/>
-      <c r="Z7"/>
-      <c r="AA7"/>
-      <c r="AB7"/>
-      <c r="AC7"/>
-      <c r="AD7"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-      <c r="K8"/>
-      <c r="L8"/>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
-      <c r="Q8"/>
-      <c r="R8"/>
-      <c r="W8"/>
-      <c r="X8"/>
-      <c r="Y8"/>
-      <c r="Z8"/>
-      <c r="AA8"/>
-      <c r="AB8"/>
-      <c r="AC8"/>
-      <c r="AD8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix layout transport,handling, add page exchange rate, allow user transport can create price table
</commit_message>
<xml_diff>
--- a/src/ExcelFile/TransportTemplate/TemplateImportTransport.xlsx
+++ b/src/ExcelFile/TransportTemplate/TemplateImportTransport.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
   <si>
     <t>Loại Vận Đơn</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>Reuse Cont</t>
+  </si>
+  <si>
+    <t>NCC</t>
+  </si>
+  <si>
+    <t>Đơn Vị Vận Tải</t>
   </si>
 </sst>
 </file>
@@ -279,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -307,6 +313,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC44"/>
+  <dimension ref="A1:AD44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA16" sqref="AA16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,9 +632,10 @@
     <col min="27" max="27" width="23.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="10" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
@@ -714,8 +723,11 @@
       <c r="AC1" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD1" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -803,8 +815,11 @@
       <c r="AC2" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD2" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -831,7 +846,7 @@
       <c r="AB3" s="14"/>
       <c r="AC3" s="14"/>
     </row>
-    <row r="4" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -858,7 +873,7 @@
       <c r="AB4" s="14"/>
       <c r="AC4" s="14"/>
     </row>
-    <row r="5" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -885,7 +900,7 @@
       <c r="AB5" s="14"/>
       <c r="AC5" s="14"/>
     </row>
-    <row r="6" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -912,7 +927,7 @@
       <c r="AB6" s="14"/>
       <c r="AC6" s="14"/>
     </row>
-    <row r="7" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -943,7 +958,7 @@
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
     </row>
-    <row r="8" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -974,7 +989,7 @@
       <c r="AB8" s="7"/>
       <c r="AC8" s="7"/>
     </row>
-    <row r="9" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1005,7 +1020,7 @@
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
     </row>
-    <row r="10" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1036,7 +1051,7 @@
       <c r="AB10" s="7"/>
       <c r="AC10" s="7"/>
     </row>
-    <row r="11" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1067,7 +1082,7 @@
       <c r="AB11" s="7"/>
       <c r="AC11" s="7"/>
     </row>
-    <row r="12" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1098,7 +1113,7 @@
       <c r="AB12" s="7"/>
       <c r="AC12" s="7"/>
     </row>
-    <row r="13" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -1129,7 +1144,7 @@
       <c r="AB13" s="7"/>
       <c r="AC13" s="7"/>
     </row>
-    <row r="14" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -1160,7 +1175,7 @@
       <c r="AB14" s="7"/>
       <c r="AC14" s="7"/>
     </row>
-    <row r="15" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1191,7 +1206,7 @@
       <c r="AB15" s="7"/>
       <c r="AC15" s="7"/>
     </row>
-    <row r="16" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>

</xml_diff>